<commit_message>
data fix, penultimate replication
</commit_message>
<xml_diff>
--- a/data/original/IISS_equipdata_1961.xlsx
+++ b/data/original/IISS_equipdata_1961.xlsx
@@ -221,15 +221,15 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="6" max="6" width="17.86"/>
-    <col customWidth="1" min="7" max="7" width="22.0"/>
-    <col customWidth="1" min="12" max="12" width="31.71"/>
-    <col customWidth="1" min="13" max="13" width="11.14"/>
-    <col customWidth="1" min="14" max="14" width="26.57"/>
-    <col customWidth="1" min="15" max="15" width="10.71"/>
+    <col customWidth="1" min="1" max="1" width="6.0"/>
+    <col customWidth="1" min="6" max="6" width="15.63"/>
+    <col customWidth="1" min="7" max="7" width="19.25"/>
+    <col customWidth="1" min="12" max="12" width="27.75"/>
+    <col customWidth="1" min="13" max="13" width="9.75"/>
+    <col customWidth="1" min="14" max="14" width="23.25"/>
+    <col customWidth="1" min="15" max="15" width="9.38"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>